<commit_message>
Ue  + moyenne par competence
</commit_message>
<xml_diff>
--- a/data/exemple.xlsx
+++ b/data/exemple.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="33">
   <si>
     <t>codenip</t>
   </si>
@@ -32,6 +32,12 @@
     <t>promotion</t>
   </si>
   <si>
+    <t>Compétence 1</t>
+  </si>
+  <si>
+    <t>Compétence 2</t>
+  </si>
+  <si>
     <t>Etudiant 1</t>
   </si>
   <si>
@@ -98,12 +104,6 @@
     <t>Promo 5</t>
   </si>
   <si>
-    <t>Compétence 1</t>
-  </si>
-  <si>
-    <t>Compétence 2</t>
-  </si>
-  <si>
     <t>Compétence 3</t>
   </si>
   <si>
@@ -111,6 +111,9 @@
   </si>
   <si>
     <t>Compétence 5</t>
+  </si>
+  <si>
+    <t>1/1</t>
   </si>
 </sst>
 </file>
@@ -450,7 +453,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:K6"/>
+  <dimension ref="A1:P6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,7 +461,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:16">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -475,10 +478,10 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
-        <v>27</v>
+        <v>5</v>
       </c>
       <c r="H1" t="s">
-        <v>28</v>
+        <v>6</v>
       </c>
       <c r="I1" t="s">
         <v>29</v>
@@ -490,7 +493,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:16">
       <c r="A2">
         <v>1</v>
       </c>
@@ -498,25 +501,37 @@
         <v>12345</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F2" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="G2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="H2" t="s">
-        <v>9</v>
+        <v>11</v>
+      </c>
+      <c r="M2" t="s">
+        <v>32</v>
+      </c>
+      <c r="N2">
+        <v>17</v>
+      </c>
+      <c r="O2">
+        <v>17.5</v>
+      </c>
+      <c r="P2">
+        <v>15.5</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:16">
       <c r="A3">
         <v>2</v>
       </c>
@@ -524,22 +539,22 @@
         <v>67890</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" t="s">
         <v>11</v>
       </c>
-      <c r="E3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G3" t="s">
-        <v>9</v>
-      </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:16">
       <c r="A4">
         <v>3</v>
       </c>
@@ -547,22 +562,22 @@
         <v>54321</v>
       </c>
       <c r="C4" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D4" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E4" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F4" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:16">
       <c r="A5">
         <v>4</v>
       </c>
@@ -570,19 +585,19 @@
         <v>98765</v>
       </c>
       <c r="C5" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D5" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E5" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="F5" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:16">
       <c r="A6">
         <v>5</v>
       </c>
@@ -590,16 +605,16 @@
         <v>13579</v>
       </c>
       <c r="C6" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D6" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E6" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="F6" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Debut du style du excel
</commit_message>
<xml_diff>
--- a/data/exemple.xlsx
+++ b/data/exemple.xlsx
@@ -15,7 +15,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="34">
+  <si>
+    <t>idetudiant</t>
+  </si>
   <si>
     <t>codenip</t>
   </si>
@@ -121,7 +124,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <b val="0"/>
       <i val="0"/>
@@ -131,13 +134,34 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <b val="1"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00FF00"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -152,8 +176,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0"/>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="0" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0"/>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="2" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="0"/>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="3" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -456,41 +483,44 @@
   <dimension ref="A1:P6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" spans="1:16">
-      <c r="B1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="I1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="K1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:16">
@@ -501,25 +531,28 @@
         <v>12345</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" t="s">
         <v>11</v>
       </c>
-      <c r="H2" t="s">
-        <v>11</v>
-      </c>
+      <c r="G2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
       <c r="M2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="N2">
         <v>17</v>
@@ -539,20 +572,24 @@
         <v>67890</v>
       </c>
       <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3" t="s">
-        <v>15</v>
-      </c>
-      <c r="G3" t="s">
-        <v>11</v>
-      </c>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
     </row>
     <row r="4" spans="1:16">
       <c r="A4">
@@ -562,20 +599,24 @@
         <v>54321</v>
       </c>
       <c r="C4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G4" t="s">
         <v>20</v>
       </c>
+      <c r="G4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
     </row>
     <row r="5" spans="1:16">
       <c r="A5">
@@ -585,17 +626,22 @@
         <v>98765</v>
       </c>
       <c r="C5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F5" t="s">
-        <v>24</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
     </row>
     <row r="6" spans="1:16">
       <c r="A6">
@@ -605,17 +651,22 @@
         <v>13579</v>
       </c>
       <c r="C6" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D6" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F6" t="s">
-        <v>28</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
     </row>
   </sheetData>
   <printOptions gridLines="false" gridLinesSet="true"/>

</xml_diff>

<commit_message>
Excel fini (sauf cursus mais tkt)
</commit_message>
<xml_diff>
--- a/data/exemple.xlsx
+++ b/data/exemple.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="53">
   <si>
     <t>Code NIP</t>
   </si>
@@ -101,7 +101,49 @@
     <t>Minime</t>
   </si>
   <si>
-    <t>BUT1</t>
+    <t>BUT 1</t>
+  </si>
+  <si>
+    <t>C1</t>
+  </si>
+  <si>
+    <t>C2</t>
+  </si>
+  <si>
+    <t>C3</t>
+  </si>
+  <si>
+    <t>C4</t>
+  </si>
+  <si>
+    <t>C5</t>
+  </si>
+  <si>
+    <t>C6</t>
+  </si>
+  <si>
+    <t>SEMESTRE 3</t>
+  </si>
+  <si>
+    <t>ADM</t>
+  </si>
+  <si>
+    <t>AJ</t>
+  </si>
+  <si>
+    <t>CMP</t>
+  </si>
+  <si>
+    <t>ADSUP</t>
+  </si>
+  <si>
+    <t>UE DU S3</t>
+  </si>
+  <si>
+    <t>UE</t>
+  </si>
+  <si>
+    <t>Moyenne</t>
   </si>
   <si>
     <t>COMP001</t>
@@ -122,19 +164,16 @@
     <t>COMP006</t>
   </si>
   <si>
-    <t>BUT2</t>
-  </si>
-  <si>
-    <t>ADM</t>
-  </si>
-  <si>
-    <t>AJ</t>
-  </si>
-  <si>
-    <t>CMP</t>
-  </si>
-  <si>
-    <t>ADSUP</t>
+    <t>4/6</t>
+  </si>
+  <si>
+    <t>0/6</t>
+  </si>
+  <si>
+    <t>6/6</t>
+  </si>
+  <si>
+    <t>0/0</t>
   </si>
 </sst>
 </file>
@@ -162,7 +201,7 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -181,6 +220,12 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFff8000"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -194,11 +239,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0"/>
     <xf xfId="0" fontId="1" numFmtId="0" fillId="0" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0"/>
     <xf xfId="0" fontId="0" numFmtId="0" fillId="2" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="0"/>
     <xf xfId="0" fontId="0" numFmtId="0" fillId="3" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="0"/>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="4" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -498,10 +544,10 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:R17"/>
+  <dimension ref="A1:Z17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="R11" sqref="R11"/>
+      <selection activeCell="S17" sqref="S17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -522,17 +568,28 @@
     <col min="16" max="16" width="12" customWidth="true" style="0"/>
     <col min="17" max="17" width="12" customWidth="true" style="0"/>
     <col min="18" max="18" width="12" customWidth="true" style="0"/>
+    <col min="19" max="19" width="7" customWidth="true" style="0"/>
+    <col min="20" max="20" width="12" customWidth="true" style="0"/>
+    <col min="21" max="21" width="12" customWidth="true" style="0"/>
+    <col min="22" max="22" width="12" customWidth="true" style="0"/>
+    <col min="23" max="23" width="12" customWidth="true" style="0"/>
+    <col min="24" max="24" width="12" customWidth="true" style="0"/>
+    <col min="25" max="25" width="12" customWidth="true" style="0"/>
+    <col min="26" max="26" width="12" customWidth="true" style="0"/>
   </cols>
   <sheetData>
-    <row r="7" spans="1:18">
+    <row r="7" spans="1:26">
       <c r="G7" s="1" t="s">
         <v>28</v>
       </c>
       <c r="M7" s="1" t="s">
         <v>35</v>
       </c>
+      <c r="S7" s="1" t="s">
+        <v>40</v>
+      </c>
     </row>
-    <row r="8" spans="1:18">
+    <row r="8" spans="1:26">
       <c r="A8" s="1" t="s">
         <v>0</v>
       </c>
@@ -581,8 +638,32 @@
       <c r="R8" s="1" t="s">
         <v>34</v>
       </c>
+      <c r="S8" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="T8" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="U8" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="V8" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="W8" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="X8" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="Y8" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="Z8" s="1" t="s">
+        <v>48</v>
+      </c>
     </row>
-    <row r="9" spans="1:18">
+    <row r="9" spans="1:26">
       <c r="A9">
         <v>1001</v>
       </c>
@@ -616,8 +697,8 @@
       <c r="M9" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="N9" s="3" t="s">
-        <v>37</v>
+      <c r="N9" s="2" t="s">
+        <v>36</v>
       </c>
       <c r="O9" s="2" t="s">
         <v>38</v>
@@ -631,8 +712,32 @@
       <c r="R9" s="2" t="s">
         <v>36</v>
       </c>
+      <c r="S9" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="T9">
+        <v>11</v>
+      </c>
+      <c r="U9" s="2">
+        <v>13.83</v>
+      </c>
+      <c r="V9" s="2">
+        <v>11.33</v>
+      </c>
+      <c r="W9" s="3">
+        <v>8.5</v>
+      </c>
+      <c r="X9" s="2">
+        <v>15.17</v>
+      </c>
+      <c r="Y9" s="2">
+        <v>13.83</v>
+      </c>
+      <c r="Z9" s="3">
+        <v>8.83</v>
+      </c>
     </row>
-    <row r="10" spans="1:18">
+    <row r="10" spans="1:26">
       <c r="A10">
         <v>1002</v>
       </c>
@@ -669,20 +774,44 @@
       <c r="N10" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="O10" s="3" t="s">
-        <v>37</v>
+      <c r="O10" s="2" t="s">
+        <v>36</v>
       </c>
       <c r="P10" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="Q10" s="3" t="s">
-        <v>37</v>
+      <c r="Q10" s="2" t="s">
+        <v>36</v>
       </c>
       <c r="R10" s="2" t="s">
         <v>36</v>
       </c>
+      <c r="S10" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="T10">
+        <v>7</v>
+      </c>
+      <c r="U10" s="3">
+        <v>8.13</v>
+      </c>
+      <c r="V10" s="3">
+        <v>6.6</v>
+      </c>
+      <c r="W10" s="3">
+        <v>5.47</v>
+      </c>
+      <c r="X10" s="3">
+        <v>8.8</v>
+      </c>
+      <c r="Y10" s="3">
+        <v>8.13</v>
+      </c>
+      <c r="Z10" s="3">
+        <v>7.47</v>
+      </c>
     </row>
-    <row r="11" spans="1:18">
+    <row r="11" spans="1:26">
       <c r="A11">
         <v>1003</v>
       </c>
@@ -731,8 +860,32 @@
       <c r="R11" s="2" t="s">
         <v>36</v>
       </c>
+      <c r="S11" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="T11">
+        <v>17</v>
+      </c>
+      <c r="U11" s="2">
+        <v>17.53</v>
+      </c>
+      <c r="V11" s="2">
+        <v>15.87</v>
+      </c>
+      <c r="W11" s="2">
+        <v>17.2</v>
+      </c>
+      <c r="X11" s="2">
+        <v>16.87</v>
+      </c>
+      <c r="Y11" s="2">
+        <v>17.53</v>
+      </c>
+      <c r="Z11" s="2">
+        <v>18.2</v>
+      </c>
     </row>
-    <row r="12" spans="1:18">
+    <row r="12" spans="1:26">
       <c r="A12">
         <v>1004</v>
       </c>
@@ -745,8 +898,14 @@
       <c r="D12" t="s">
         <v>15</v>
       </c>
+      <c r="S12" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="T12">
+        <v>0</v>
+      </c>
     </row>
-    <row r="13" spans="1:18">
+    <row r="13" spans="1:26">
       <c r="A13">
         <v>1005</v>
       </c>
@@ -759,8 +918,14 @@
       <c r="D13" t="s">
         <v>18</v>
       </c>
+      <c r="S13" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="T13">
+        <v>0</v>
+      </c>
     </row>
-    <row r="14" spans="1:18">
+    <row r="14" spans="1:26">
       <c r="A14">
         <v>1006</v>
       </c>
@@ -773,8 +938,14 @@
       <c r="D14" t="s">
         <v>21</v>
       </c>
+      <c r="S14" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="T14">
+        <v>0</v>
+      </c>
     </row>
-    <row r="15" spans="1:18">
+    <row r="15" spans="1:26">
       <c r="A15">
         <v>1007</v>
       </c>
@@ -787,8 +958,14 @@
       <c r="D15" t="s">
         <v>18</v>
       </c>
+      <c r="S15" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="T15">
+        <v>0</v>
+      </c>
     </row>
-    <row r="16" spans="1:18">
+    <row r="16" spans="1:26">
       <c r="A16">
         <v>1008</v>
       </c>
@@ -801,8 +978,14 @@
       <c r="D16" t="s">
         <v>18</v>
       </c>
+      <c r="S16" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="T16">
+        <v>0</v>
+      </c>
     </row>
-    <row r="17" spans="1:18">
+    <row r="17" spans="1:26">
       <c r="A17">
         <v>1009</v>
       </c>
@@ -814,12 +997,19 @@
       </c>
       <c r="D17" t="s">
         <v>18</v>
+      </c>
+      <c r="S17" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="T17">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <mergeCells>
     <mergeCell ref="G7:L7"/>
     <mergeCell ref="M7:R7"/>
+    <mergeCell ref="S7:Z7"/>
   </mergeCells>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>